<commit_message>
Perft - Character section
</commit_message>
<xml_diff>
--- a/Perft.xlsx
+++ b/Perft.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="48">
   <si>
     <t>Initial Testcase, Debug Mode</t>
   </si>
@@ -137,6 +137,27 @@
   </si>
   <si>
     <t>20,2,995</t>
+  </si>
+  <si>
+    <t>After fixing character section</t>
+  </si>
+  <si>
+    <t>1,20,528</t>
+  </si>
+  <si>
+    <t>20,2,984</t>
+  </si>
+  <si>
+    <t>1,20,519</t>
+  </si>
+  <si>
+    <t>20,2,989</t>
+  </si>
+  <si>
+    <t>1,20,516</t>
+  </si>
+  <si>
+    <t>20,2,985</t>
   </si>
 </sst>
 </file>
@@ -478,19 +499,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G25"/>
+  <dimension ref="B3:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="13" width="29.42578125" customWidth="1"/>
+    <col min="2" max="7" width="29.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" customWidth="1"/>
+    <col min="9" max="13" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -509,8 +532,11 @@
       <c r="G3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -529,8 +555,11 @@
       <c r="G5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -549,8 +578,11 @@
       <c r="G6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>9</v>
       </c>
@@ -569,8 +601,11 @@
       <c r="G7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>2</v>
       </c>
@@ -589,8 +624,11 @@
       <c r="G8" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>1</v>
       </c>
@@ -609,8 +647,11 @@
       <c r="G9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -629,8 +670,11 @@
       <c r="G10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>2</v>
       </c>
@@ -646,8 +690,11 @@
       <c r="G11" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>1</v>
       </c>
@@ -663,8 +710,11 @@
       <c r="G12" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -683,8 +733,11 @@
       <c r="G13" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>2</v>
       </c>
@@ -703,8 +756,11 @@
       <c r="G14" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>1</v>
       </c>
@@ -723,8 +779,11 @@
       <c r="G15" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>12</v>
       </c>
@@ -743,8 +802,11 @@
       <c r="G16" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>2</v>
       </c>
@@ -763,8 +825,11 @@
       <c r="G17" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>1</v>
       </c>
@@ -783,8 +848,11 @@
       <c r="G18" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>13</v>
       </c>
@@ -800,8 +868,11 @@
       <c r="G19" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>2</v>
       </c>
@@ -820,8 +891,11 @@
       <c r="G20" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>1</v>
       </c>
@@ -840,8 +914,11 @@
       <c r="G21" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>14</v>
       </c>
@@ -860,18 +937,21 @@
       <c r="G22" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
cleanups. Move Update() calls outside loops, zero-init buffers, address all outstanding compiler warnings.
</commit_message>
<xml_diff>
--- a/Perft.xlsx
+++ b/Perft.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="55">
   <si>
     <t>Initial Testcase, Debug Mode</t>
   </si>
@@ -158,6 +158,27 @@
   </si>
   <si>
     <t>20,2,985</t>
+  </si>
+  <si>
+    <t>After cleanup</t>
+  </si>
+  <si>
+    <t>1,20,511</t>
+  </si>
+  <si>
+    <t>20,2,966</t>
+  </si>
+  <si>
+    <t>1,20,500</t>
+  </si>
+  <si>
+    <t>20,2,958</t>
+  </si>
+  <si>
+    <t>1,20,495</t>
+  </si>
+  <si>
+    <t>20,2,955</t>
   </si>
 </sst>
 </file>
@@ -499,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:I25"/>
+  <dimension ref="B3:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,7 +534,7 @@
     <col min="9" max="13" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -535,8 +556,11 @@
       <c r="I3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -558,8 +582,11 @@
       <c r="I5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -581,8 +608,11 @@
       <c r="I6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>9</v>
       </c>
@@ -604,8 +634,11 @@
       <c r="I7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>2</v>
       </c>
@@ -627,8 +660,11 @@
       <c r="I8" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>1</v>
       </c>
@@ -650,8 +686,11 @@
       <c r="I9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -673,8 +712,11 @@
       <c r="I10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>2</v>
       </c>
@@ -693,8 +735,11 @@
       <c r="I11" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>1</v>
       </c>
@@ -713,8 +758,11 @@
       <c r="I12" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -736,8 +784,11 @@
       <c r="I13" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>2</v>
       </c>
@@ -759,8 +810,11 @@
       <c r="I14" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>1</v>
       </c>
@@ -782,8 +836,11 @@
       <c r="I15" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>12</v>
       </c>
@@ -805,8 +862,11 @@
       <c r="I16" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>2</v>
       </c>
@@ -828,8 +888,11 @@
       <c r="I17" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>1</v>
       </c>
@@ -851,8 +914,11 @@
       <c r="I18" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>13</v>
       </c>
@@ -871,8 +937,11 @@
       <c r="I19" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>2</v>
       </c>
@@ -894,8 +963,11 @@
       <c r="I20" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>1</v>
       </c>
@@ -917,8 +989,11 @@
       <c r="I21" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>14</v>
       </c>
@@ -940,18 +1015,21 @@
       <c r="I22" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>8</v>
       </c>

</xml_diff>